<commit_message>
Tested initial data-dictionary classification against system function points to create refined data-dictionary classification
</commit_message>
<xml_diff>
--- a/object-analysis.xlsx
+++ b/object-analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>PaginationDevice</t>
   </si>
@@ -64,6 +64,54 @@
   </si>
   <si>
     <t>NewsTickerLoadsFeed</t>
+  </si>
+  <si>
+    <t>System Function Points</t>
+  </si>
+  <si>
+    <t>Must show exactly one item from the feed at a time</t>
+  </si>
+  <si>
+    <t>Must accept feed in JSON format</t>
+  </si>
+  <si>
+    <t>Related to system function point</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1, 2,3</t>
+  </si>
+  <si>
+    <t>3,</t>
+  </si>
+  <si>
+    <t>0,</t>
+  </si>
+  <si>
+    <t>Pagination device should conform to GEL</t>
+  </si>
+  <si>
+    <t>2?</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>NewsFeedDidLoad</t>
+  </si>
+  <si>
+    <t>NewsTickerButton?</t>
+  </si>
+  <si>
+    <t>NewsTickerItem?</t>
+  </si>
+  <si>
+    <t>NewsTickerBeginNavigation</t>
   </si>
 </sst>
 </file>
@@ -95,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -103,13 +151,137 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,93 +583,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="B24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>